<commit_message>
working version with 64 values
</commit_message>
<xml_diff>
--- a/assignment/meresek.xlsx
+++ b/assignment/meresek.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au088680\Documents\c_sdk_220203\excersises\assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC846780-0AAA-48C0-A588-21CAFDCB478A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1737DC41-2381-4148-ABC4-94D6917123F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F4E77CD5-58E2-4AFF-A0D3-737FAD77D6AF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="31">
   <si>
     <t>number of groups</t>
   </si>
@@ -102,16 +102,50 @@
   </si>
   <si>
     <t>number of samples in both buffers</t>
+  </si>
+  <si>
+    <t>vector</t>
+  </si>
+  <si>
+    <t>short4</t>
+  </si>
+  <si>
+    <t>1.193</t>
+  </si>
+  <si>
+    <t>30.000</t>
+  </si>
+  <si>
+    <t>short8</t>
+  </si>
+  <si>
+    <t>1.401</t>
+  </si>
+  <si>
+    <t>short16</t>
+  </si>
+  <si>
+    <t>1.367</t>
+  </si>
+  <si>
+    <t>with buffer mapping</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <charset val="238"/>
@@ -145,7 +179,35 @@
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="9">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -156,6 +218,35 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D5F9F067-B023-4915-AF33-1602BE23BD52}" name="Táblázat1" displayName="Táblázat1" ref="A1:F10" totalsRowShown="0">
+  <autoFilter ref="A1:F10" xr:uid="{D5F9F067-B023-4915-AF33-1602BE23BD52}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{2939D1A4-080B-4152-A056-9E6339060C0F}" name="number of samples in both buffers" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{6807C98C-706E-4F72-8341-A48F726F554D}" name="number of groups" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{1C57CA33-0BB9-40EA-BDA9-A17D095B2681}" name="Kernel execution time" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{82936C23-3EB6-4E6C-92E9-1628957FE520}" name="Host waiting time" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{45019E4C-B939-42AB-8F49-E6AAA899494C}" name="Total processing time" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{1069B895-C7B8-4FEF-B237-1A039DC423AC}" name="with buffer mapping" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{FA33BB6C-A07E-463D-B026-BCFD8EC7AE7C}" name="Táblázat2" displayName="Táblázat2" ref="A12:E15" totalsRowShown="0">
+  <autoFilter ref="A12:E15" xr:uid="{FA33BB6C-A07E-463D-B026-BCFD8EC7AE7C}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{6BCA5BE3-3D43-4FD3-A8EF-FF0558448A14}" name="vector"/>
+    <tableColumn id="2" xr3:uid="{3029CDBE-984E-4C79-A5BB-911C89051A5E}" name="number of groups"/>
+    <tableColumn id="3" xr3:uid="{C0215D2D-D5C6-4569-AF00-50ADD068B42D}" name="Kernel execution time" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{5CE4A6E9-DDA5-45D0-81D2-8094E8E638D2}" name="Host waiting time" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{69722401-C6FE-4B81-A517-36104CC9AECE}" name="Total processing time" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -475,22 +566,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{388FD600-D880-4719-929A-D8EE2507AD02}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -506,8 +598,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>4</v>
       </c>
@@ -523,8 +618,11 @@
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>8</v>
       </c>
@@ -540,8 +638,11 @@
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>16</v>
       </c>
@@ -557,8 +658,11 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>32</v>
       </c>
@@ -574,8 +678,11 @@
       <c r="E5" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>64</v>
       </c>
@@ -591,8 +698,9 @@
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="1"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>128</v>
       </c>
@@ -608,8 +716,9 @@
       <c r="E7" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>256</v>
       </c>
@@ -625,8 +734,9 @@
       <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>512</v>
       </c>
@@ -642,8 +752,9 @@
       <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1024</v>
       </c>
@@ -659,8 +770,82 @@
       <c r="E10" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1639375</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1">
+        <v>819687</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1">
+        <v>409843</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="2">
+    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>